<commit_message>
agregamos datos al formato del psp
</commit_message>
<xml_diff>
--- a/Formato PSP Arteaga_libreta.xlsx
+++ b/Formato PSP Arteaga_libreta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerli\Desktop\Repositorios\Arteaga_libreta-de-direcciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90525EE6-2A49-4CC7-A179-CB373F9E1F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D44127-C77D-43F0-8435-05EA3A87BD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="1" activeTab="4" xr2:uid="{5C91324D-6205-4AF6-A214-4DE2B566EAE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="3" activeTab="6" xr2:uid="{5C91324D-6205-4AF6-A214-4DE2B566EAE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduccion PSP" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="126">
   <si>
     <t>ESTANDARES DE CODIFICACIÓN</t>
   </si>
@@ -486,12 +486,6 @@
     <t>Usa formato 24 horas</t>
   </si>
   <si>
-    <t>Ver Pág 18 de DMDS_U1.PDF</t>
-  </si>
-  <si>
-    <t>Ver Pág 20 de DMDS_U1.PDF</t>
-  </si>
-  <si>
     <t>Encontrado (Introducido/Inyectado)
 (Fase de PSP)</t>
   </si>
@@ -500,7 +494,19 @@
  (Fase de PSP)</t>
   </si>
   <si>
-    <t>Ver Pág 22 de DMDS_U1.PDF</t>
+    <t>Gerly Daniel Arteaga bernal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose Antonio Vergara Camacho </t>
+  </si>
+  <si>
+    <t>22 de mayo de 2024</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Gerly Daniel Arteaga Bernal</t>
   </si>
 </sst>
 </file>
@@ -751,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -813,23 +819,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -849,7 +840,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -864,23 +867,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -892,6 +880,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -918,6 +912,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -928,6 +934,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -936,9 +945,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588BB31E-4CEC-469F-B8F6-09292E0004A4}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1407,170 +1417,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="55.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" ht="201.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="29" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="150.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -1582,16 +1602,6 @@
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1612,102 +1622,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:9" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="28" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
@@ -1717,11 +1732,6 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1744,16 +1754,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1777,20 +1787,20 @@
       <c r="AC1" s="5"/>
     </row>
     <row r="2" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -1814,14 +1824,14 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1845,20 +1855,20 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="54"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -1882,18 +1892,18 @@
       <c r="AC4" s="5"/>
     </row>
     <row r="5" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1917,18 +1927,18 @@
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1953,17 +1963,17 @@
     </row>
     <row r="7" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1988,17 +1998,17 @@
     </row>
     <row r="8" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -2023,17 +2033,17 @@
     </row>
     <row r="9" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="44"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -2058,17 +2068,17 @@
     </row>
     <row r="10" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -2092,18 +2102,18 @@
       <c r="AC10" s="5"/>
     </row>
     <row r="11" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -2128,17 +2138,17 @@
     </row>
     <row r="12" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="59"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -4789,6 +4799,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -4801,16 +4821,6 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4818,26 +4828,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35175C74-1589-4401-92EC-A60D5C8F9D38}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>123</v>
-      </c>
-    </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="60" t="s">
         <v>45</v>
@@ -4851,23 +4856,31 @@
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="61"/>
+      <c r="B5" s="61" t="s">
+        <v>121</v>
+      </c>
       <c r="C5" s="61"/>
       <c r="D5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="20" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="61" t="s">
+        <v>122</v>
+      </c>
       <c r="C6" s="61"/>
       <c r="D6" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="20" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
@@ -5107,25 +5120,23 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5164,7 +5175,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="A6" s="67">
+        <v>45434</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -5229,10 +5242,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1E9371-A978-4959-97B1-907507EF065D}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5241,206 +5254,206 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65" t="s">
+      <c r="C6" s="66"/>
+      <c r="D6" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>10</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="66" t="s">
+      <c r="C7" s="64"/>
+      <c r="D7" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>20</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="66" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>30</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="66" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>40</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="66" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>50</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="66" t="s">
+      <c r="C11" s="64"/>
+      <c r="D11" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>60</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="66" t="s">
+      <c r="C12" s="64"/>
+      <c r="D12" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>70</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="66" t="s">
+      <c r="C13" s="64"/>
+      <c r="D13" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>80</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="66" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>90</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="66" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="64"/>
+      <c r="D16" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="61"/>
+      <c r="B18" s="61" t="s">
+        <v>125</v>
+      </c>
       <c r="C18" s="61"/>
       <c r="D18" s="61"/>
       <c r="E18" s="61"/>
       <c r="F18" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="G18" s="68">
+        <v>45434</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G19" s="12"/>
@@ -5456,10 +5469,10 @@
         <v>89</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>81</v>
@@ -5470,7 +5483,9 @@
     </row>
     <row r="21" spans="1:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -5514,7 +5529,9 @@
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -5558,7 +5575,9 @@
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -5602,7 +5621,9 @@
     </row>
     <row r="35" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -5621,20 +5642,55 @@
       <c r="F37" s="61"/>
       <c r="G37" s="61"/>
     </row>
+    <row r="38" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3">
+        <v>5</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
+  <mergeCells count="29">
+    <mergeCell ref="B41:G41"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B37:G37"/>
@@ -5651,12 +5707,33 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C3FE6271BEA2C45BD053C062D34DAB8" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8c4fe01e16a7d30497b436951f273215">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="302a697f-c05b-4e64-9398-25fe8623ee8c" xmlns:ns4="0f6e5129-90bf-4ef3-b1b4-c0d43a9656e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00a4e6a6de0be021f3e45b28a1c15569" ns3:_="" ns4:_="">
     <xsd:import namespace="302a697f-c05b-4e64-9398-25fe8623ee8c"/>
@@ -5909,15 +5986,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5927,6 +5995,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2504083-5C3D-4649-9EFF-1D07A6C3996D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E14591D-47D5-498B-B18C-CA60E582947C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5941,14 +6017,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2504083-5C3D-4649-9EFF-1D07A6C3996D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>